<commit_message>
AutoCommit_4 июля 2023 г. 10:03:53_SibNout2020
</commit_message>
<xml_diff>
--- a/3ПКС-120/3ПКС-120_Сети.xlsx
+++ b/3ПКС-120/3ПКС-120_Сети.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\3ПКС-120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2756B320-AF25-4AFC-AED3-6C48DB252C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E092CAC-FDE4-4BEC-8551-361DDC29EFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,7 +553,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T14" sqref="T14"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1244,8 +1244,12 @@
         <v>10</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5">
+        <v>5</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5">
         <v>5</v>
@@ -1284,7 +1288,7 @@
       <c r="U14" s="5"/>
       <c r="V14">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_4 июля 2023 г. 14:52:25_SibNout2020
</commit_message>
<xml_diff>
--- a/3ПКС-120/3ПКС-120_Сети.xlsx
+++ b/3ПКС-120/3ПКС-120_Сети.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\3ПКС-120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E092CAC-FDE4-4BEC-8551-361DDC29EFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7049BB3-FCC3-45A4-97AC-640AFFF6EF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,7 +553,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="N4" sqref="N4:N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -644,7 +644,9 @@
       <c r="E4" s="3">
         <v>5</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
       <c r="G4" s="5"/>
       <c r="H4" s="3">
         <v>5</v>
@@ -656,11 +658,15 @@
       <c r="K4" s="4">
         <v>5</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
       <c r="M4" s="3">
         <v>5</v>
       </c>
-      <c r="N4" s="5"/>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
       <c r="O4" s="5"/>
       <c r="P4" s="3">
         <v>5</v>
@@ -696,7 +702,9 @@
       <c r="E5" s="3">
         <v>5</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
       <c r="G5" s="3">
         <v>5</v>
       </c>
@@ -772,11 +780,15 @@
       <c r="K6" s="4">
         <v>5</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
       <c r="M6" s="3">
         <v>5</v>
       </c>
-      <c r="N6" s="5"/>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
       <c r="O6" s="3">
         <v>5</v>
       </c>
@@ -838,7 +850,9 @@
       <c r="M7" s="3">
         <v>5</v>
       </c>
-      <c r="N7" s="5"/>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
       <c r="O7" s="3">
         <v>5</v>
       </c>
@@ -874,15 +888,21 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
       <c r="I8" s="3">
         <v>5</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
+      <c r="L8" s="6">
+        <v>0</v>
+      </c>
       <c r="M8" s="5"/>
       <c r="N8" s="3">
         <v>5</v>
@@ -924,7 +944,9 @@
       <c r="E9" s="5">
         <v>5</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
       <c r="G9" s="3">
         <v>5</v>
       </c>
@@ -1250,11 +1272,15 @@
       <c r="E14" s="5">
         <v>5</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
       <c r="G14" s="5">
         <v>5</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5">
         <v>5</v>
@@ -1375,7 +1401,9 @@
       <c r="E16" s="3">
         <v>5</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
       <c r="G16" s="3">
         <v>5</v>
       </c>
@@ -1565,9 +1593,13 @@
       <c r="E19" s="3">
         <v>5</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
       <c r="I19" s="5"/>
       <c r="J19" s="3">
         <v>5</v>
@@ -1575,11 +1607,15 @@
       <c r="K19" s="4">
         <v>5</v>
       </c>
-      <c r="L19" s="6"/>
+      <c r="L19" s="6">
+        <v>0</v>
+      </c>
       <c r="M19" s="3">
         <v>5</v>
       </c>
-      <c r="N19" s="5"/>
+      <c r="N19" s="5">
+        <v>0</v>
+      </c>
       <c r="O19" s="5"/>
       <c r="P19" s="3">
         <v>5</v>
@@ -1627,9 +1663,13 @@
       <c r="K20" s="4">
         <v>5</v>
       </c>
-      <c r="L20" s="6"/>
+      <c r="L20" s="6">
+        <v>0</v>
+      </c>
       <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
+      <c r="N20" s="5">
+        <v>0</v>
+      </c>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
@@ -1659,13 +1699,19 @@
         <v>5</v>
       </c>
       <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
+      <c r="L21" s="6">
+        <v>0</v>
+      </c>
       <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
+      <c r="N21" s="5">
+        <v>0</v>
+      </c>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
@@ -1823,7 +1869,9 @@
       <c r="E24" s="3">
         <v>5</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
       <c r="G24" s="3">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_5 июля 2023 г. 9:39:21_SibNout2020
</commit_message>
<xml_diff>
--- a/3ПКС-120/3ПКС-120_Сети.xlsx
+++ b/3ПКС-120/3ПКС-120_Сети.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\3ПКС-120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7049BB3-FCC3-45A4-97AC-640AFFF6EF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29492A44-03F1-4485-954A-0E2DB852AAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,7 +553,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N4" sqref="N4:N25"/>
+      <selection pane="bottomRight" activeCell="T9" activeCellId="1" sqref="O9:R9 T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -938,10 +938,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="5">
-        <v>5</v>
-      </c>
-      <c r="E9" s="5">
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3">
         <v>5</v>
       </c>
       <c r="F9" s="5">
@@ -969,20 +969,20 @@
       <c r="N9" s="3">
         <v>5</v>
       </c>
-      <c r="O9" s="5">
-        <v>5</v>
-      </c>
-      <c r="P9" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q9" s="5">
+      <c r="O9" s="3">
+        <v>5</v>
+      </c>
+      <c r="P9" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="3">
         <v>6</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="3">
         <v>5</v>
       </c>
       <c r="S9" s="5"/>
-      <c r="T9" s="5">
+      <c r="T9" s="3">
         <v>5</v>
       </c>
       <c r="U9" s="5"/>
@@ -1266,49 +1266,49 @@
         <v>10</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="5">
-        <v>5</v>
-      </c>
-      <c r="E14" s="5">
+      <c r="D14" s="3">
+        <v>5</v>
+      </c>
+      <c r="E14" s="3">
         <v>5</v>
       </c>
       <c r="F14" s="5">
         <v>0</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="3">
         <v>5</v>
       </c>
       <c r="H14" s="5">
         <v>0</v>
       </c>
       <c r="I14" s="5"/>
-      <c r="J14" s="5">
-        <v>5</v>
-      </c>
-      <c r="K14" s="6">
-        <v>5</v>
-      </c>
-      <c r="L14" s="6">
+      <c r="J14" s="3">
+        <v>5</v>
+      </c>
+      <c r="K14" s="4">
+        <v>5</v>
+      </c>
+      <c r="L14" s="4">
         <v>5</v>
       </c>
       <c r="M14" s="5"/>
-      <c r="N14" s="5">
-        <v>5</v>
-      </c>
-      <c r="O14" s="5">
-        <v>5</v>
-      </c>
-      <c r="P14" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q14" s="5">
-        <v>5</v>
-      </c>
-      <c r="R14" s="5">
+      <c r="N14" s="3">
+        <v>5</v>
+      </c>
+      <c r="O14" s="3">
+        <v>5</v>
+      </c>
+      <c r="P14" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>5</v>
+      </c>
+      <c r="R14" s="3">
         <v>5</v>
       </c>
       <c r="S14" s="5"/>
-      <c r="T14" s="5">
+      <c r="T14" s="3">
         <v>5</v>
       </c>
       <c r="U14" s="5"/>

</xml_diff>